<commit_message>
Auto update on 2025-12-03 07:35:58
</commit_message>
<xml_diff>
--- a/kp_data.xlsx
+++ b/kp_data.xlsx
@@ -15636,10 +15636,10 @@
         <v>5</v>
       </c>
       <c r="D16">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E16">
-        <v>1.9</v>
+        <v>1.86</v>
       </c>
       <c r="F16">
         <v>0.05</v>
@@ -62553,7 +62553,7 @@
         <v>968</v>
       </c>
       <c r="B2429" t="s">
-        <v>963</v>
+        <v>1061</v>
       </c>
       <c r="C2429" t="s">
         <v>3503</v>

</xml_diff>

<commit_message>
Auto update on 2025-12-20 09:36:15
</commit_message>
<xml_diff>
--- a/kp_data.xlsx
+++ b/kp_data.xlsx
@@ -3531,10 +3531,10 @@
     <t>2025-07-02</t>
   </si>
   <si>
+    <t>2025-12-19</t>
+  </si>
+  <si>
     <t>2025-09-05</t>
-  </si>
-  <si>
-    <t>2025-12-19</t>
   </si>
   <si>
     <t>2025-03-20</t>
@@ -16995,10 +16995,10 @@
         <v>43</v>
       </c>
       <c r="D7">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E7">
-        <v>4.32</v>
+        <v>4.27</v>
       </c>
       <c r="F7">
         <v>0.11</v>
@@ -29506,10 +29506,10 @@
     </row>
     <row r="334" spans="1:5">
       <c r="A334" t="s">
-        <v>1138</v>
+        <v>1135</v>
       </c>
       <c r="B334" t="s">
-        <v>1130</v>
+        <v>1171</v>
       </c>
       <c r="C334" t="s">
         <v>1576</v>
@@ -29526,7 +29526,7 @@
         <v>1135</v>
       </c>
       <c r="B335" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="C335" t="s">
         <v>1577</v>
@@ -29577,7 +29577,7 @@
         <v>1135</v>
       </c>
       <c r="B338" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="C338" t="s">
         <v>1580</v>
@@ -29764,7 +29764,7 @@
         <v>1134</v>
       </c>
       <c r="B349" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C349" t="s">
         <v>1591</v>
@@ -29781,7 +29781,7 @@
         <v>1134</v>
       </c>
       <c r="B350" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C350" t="s">
         <v>1592</v>
@@ -29798,7 +29798,7 @@
         <v>1134</v>
       </c>
       <c r="B351" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C351" t="s">
         <v>1593</v>
@@ -29815,7 +29815,7 @@
         <v>1134</v>
       </c>
       <c r="B352" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C352" t="s">
         <v>1594</v>
@@ -29832,7 +29832,7 @@
         <v>1134</v>
       </c>
       <c r="B353" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C353" t="s">
         <v>1595</v>
@@ -29849,7 +29849,7 @@
         <v>1134</v>
       </c>
       <c r="B354" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C354" t="s">
         <v>1596</v>
@@ -29866,7 +29866,7 @@
         <v>1134</v>
       </c>
       <c r="B355" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C355" t="s">
         <v>1597</v>
@@ -29883,7 +29883,7 @@
         <v>1134</v>
       </c>
       <c r="B356" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C356" t="s">
         <v>1598</v>
@@ -29900,7 +29900,7 @@
         <v>1135</v>
       </c>
       <c r="B357" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C357" t="s">
         <v>1599</v>
@@ -35629,7 +35629,7 @@
         <v>1135</v>
       </c>
       <c r="B694" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C694" t="s">
         <v>1936</v>
@@ -35646,7 +35646,7 @@
         <v>1138</v>
       </c>
       <c r="B695" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C695" t="s">
         <v>1937</v>
@@ -51660,7 +51660,7 @@
         <v>1138</v>
       </c>
       <c r="B1637" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C1637" t="s">
         <v>2879</v>
@@ -53309,7 +53309,7 @@
         <v>1134</v>
       </c>
       <c r="B1734" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="C1734" t="s">
         <v>2976</v>
@@ -53751,7 +53751,7 @@
         <v>1134</v>
       </c>
       <c r="B1760" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C1760" t="s">
         <v>3002</v>
@@ -53938,7 +53938,7 @@
         <v>1138</v>
       </c>
       <c r="B1771" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C1771" t="s">
         <v>3013</v>
@@ -55723,7 +55723,7 @@
         <v>1135</v>
       </c>
       <c r="B1876" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="C1876" t="s">
         <v>3118</v>
@@ -66943,7 +66943,7 @@
         <v>1138</v>
       </c>
       <c r="B2536" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C2536" t="s">
         <v>3778</v>
@@ -67759,7 +67759,7 @@
         <v>1138</v>
       </c>
       <c r="B2584" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C2584" t="s">
         <v>3826</v>
@@ -67776,7 +67776,7 @@
         <v>1138</v>
       </c>
       <c r="B2585" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C2585" t="s">
         <v>3827</v>
@@ -67827,7 +67827,7 @@
         <v>1134</v>
       </c>
       <c r="B2588" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C2588" t="s">
         <v>3830</v>
@@ -69561,7 +69561,7 @@
         <v>1135</v>
       </c>
       <c r="B2690" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C2690" t="s">
         <v>3932</v>
@@ -69595,7 +69595,7 @@
         <v>1134</v>
       </c>
       <c r="B2692" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C2692" t="s">
         <v>3934</v>
@@ -69969,7 +69969,7 @@
         <v>1135</v>
       </c>
       <c r="B2714" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C2714" t="s">
         <v>3956</v>

</xml_diff>